<commit_message>
845 Longest Mountain in Array
</commit_message>
<xml_diff>
--- a/leetcode_questions_solved.xlsx
+++ b/leetcode_questions_solved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\job\Studies\Masters\2nd Semester\Leetcode Challenge\Data Structures and Algorithms\100DaysLeetcodeChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9569308D-9487-4F64-A179-0B0124BB2F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD2506D-EBCF-45DA-B562-A97F7AE09782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6240" windowWidth="29040" windowHeight="15720" xr2:uid="{AE498830-861B-4F35-8A74-F037B6EAC04E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AE498830-861B-4F35-8A74-F037B6EAC04E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="611">
   <si>
     <t>https://leetcode.com/problems/binary-tree-inorder-traversal/</t>
   </si>
@@ -1857,6 +1857,19 @@
   </si>
   <si>
     <t xml:space="preserve"> Pow(x,  n)</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Subtract the length of two lists to get what is there common length</t>
+  </si>
+  <si>
+    <t>Find at each node if it is boolean balanced or not
+return [balanced, 1 + max(left_depth[1], right_depth[1])]</t>
+  </si>
+  <si>
+    <t>I did in O(n2), can be possibly done in O(n)</t>
   </si>
 </sst>
 </file>
@@ -2242,3361 +2255,3383 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E6AF243-3367-49A7-8F52-7AC93B956991}">
-  <dimension ref="A1:C303"/>
+  <dimension ref="A1:D303"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A293" workbookViewId="0">
+      <selection activeCell="C299" sqref="C299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.88671875" customWidth="1"/>
     <col min="2" max="2" width="52.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.77734375" customWidth="1"/>
+    <col min="4" max="4" width="77.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>603</v>
       </c>
       <c r="B1" t="s">
         <v>604</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>94</v>
       </c>
       <c r="B2" t="s">
         <v>302</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>88</v>
       </c>
       <c r="B3" t="s">
         <v>303</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>304</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>305</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>306</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>307</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>308</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>309</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>73</v>
       </c>
       <c r="B10" t="s">
         <v>310</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>75</v>
       </c>
       <c r="B11" t="s">
         <v>311</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>70</v>
       </c>
       <c r="B12" t="s">
         <v>312</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>69</v>
       </c>
       <c r="B13" t="s">
         <v>313</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>122</v>
       </c>
       <c r="B14" t="s">
         <v>314</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>67</v>
       </c>
       <c r="B15" t="s">
         <v>315</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>371</v>
       </c>
       <c r="B16" t="s">
         <v>316</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>76</v>
       </c>
       <c r="B17" t="s">
         <v>317</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>295</v>
       </c>
       <c r="B18" t="s">
         <v>318</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>424</v>
       </c>
       <c r="B19" t="s">
         <v>319</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>143</v>
       </c>
       <c r="B20" t="s">
         <v>320</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>876</v>
       </c>
       <c r="B21" t="s">
         <v>321</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>33</v>
       </c>
       <c r="B22" t="s">
         <v>322</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>877</v>
       </c>
       <c r="B23" t="s">
         <v>323</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>292</v>
       </c>
       <c r="B24" t="s">
         <v>324</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>322</v>
       </c>
       <c r="B25" t="s">
         <v>325</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>649</v>
       </c>
       <c r="B26" t="s">
         <v>326</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>735</v>
       </c>
       <c r="B27" t="s">
         <v>327</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>724</v>
       </c>
       <c r="B28" t="s">
         <v>328</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1732</v>
       </c>
       <c r="B29" t="s">
         <v>329</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1071</v>
       </c>
       <c r="B30" t="s">
         <v>330</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>452</v>
       </c>
       <c r="B31" t="s">
         <v>331</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>435</v>
       </c>
       <c r="B32" t="s">
         <v>332</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1318</v>
       </c>
       <c r="B33" t="s">
         <v>333</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>136</v>
       </c>
       <c r="B34" t="s">
         <v>334</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>338</v>
       </c>
       <c r="B35" t="s">
         <v>335</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>714</v>
       </c>
       <c r="B36" t="s">
         <v>336</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1143</v>
       </c>
       <c r="B37" t="s">
         <v>337</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>62</v>
       </c>
       <c r="B38" t="s">
         <v>338</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1004</v>
       </c>
       <c r="B39" t="s">
         <v>339</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>643</v>
       </c>
       <c r="B40" t="s">
         <v>340</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>739</v>
       </c>
       <c r="B41" t="s">
         <v>341</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>901</v>
       </c>
       <c r="B42" t="s">
         <v>342</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>198</v>
       </c>
       <c r="B43" t="s">
         <v>343</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>746</v>
       </c>
       <c r="B44" t="s">
         <v>344</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1268</v>
       </c>
       <c r="B45" t="s">
         <v>345</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>208</v>
       </c>
       <c r="B46" t="s">
         <v>346</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1137</v>
       </c>
       <c r="B47" t="s">
         <v>347</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>162</v>
       </c>
       <c r="B48" t="s">
         <v>348</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>216</v>
       </c>
       <c r="B49" t="s">
         <v>349</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>17</v>
       </c>
       <c r="B50" t="s">
         <v>350</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>374</v>
       </c>
       <c r="B51" t="s">
         <v>351</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>215</v>
       </c>
       <c r="B52" t="s">
         <v>352</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2462</v>
       </c>
       <c r="B53" t="s">
         <v>353</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2542</v>
       </c>
       <c r="B54" t="s">
         <v>354</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2336</v>
       </c>
       <c r="B55" t="s">
         <v>355</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>399</v>
       </c>
       <c r="B56" t="s">
         <v>356</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>1466</v>
       </c>
       <c r="B57" t="s">
         <v>357</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>547</v>
       </c>
       <c r="B58" t="s">
         <v>358</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>841</v>
       </c>
       <c r="B59" t="s">
         <v>359</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>700</v>
       </c>
       <c r="B60" t="s">
         <v>360</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>72</v>
       </c>
       <c r="B61" t="s">
         <v>361</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>392</v>
       </c>
       <c r="B62" t="s">
         <v>362</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>1527</v>
       </c>
       <c r="B63" t="s">
         <v>363</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>1667</v>
       </c>
       <c r="B64" t="s">
         <v>364</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>185</v>
       </c>
       <c r="B65" t="s">
         <v>365</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>585</v>
       </c>
       <c r="B66" t="s">
         <v>366</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>602</v>
       </c>
       <c r="B67" t="s">
         <v>367</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>283</v>
       </c>
       <c r="B68" t="s">
         <v>368</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>443</v>
       </c>
       <c r="B69" t="s">
         <v>369</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>334</v>
       </c>
       <c r="B70" t="s">
         <v>370</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>151</v>
       </c>
       <c r="B71" t="s">
         <v>371</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>345</v>
       </c>
       <c r="B72" t="s">
         <v>372</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>605</v>
       </c>
       <c r="B73" t="s">
         <v>373</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="D73" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>1431</v>
       </c>
       <c r="B74" t="s">
         <v>374</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>1321</v>
       </c>
       <c r="B75" t="s">
         <v>375</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>1341</v>
       </c>
       <c r="B76" t="s">
         <v>376</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>626</v>
       </c>
       <c r="B77" t="s">
         <v>377</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>1768</v>
       </c>
       <c r="B78" t="s">
         <v>378</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>1978</v>
       </c>
       <c r="B79" t="s">
         <v>379</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>1907</v>
       </c>
       <c r="B80" t="s">
         <v>380</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="D80" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>1204</v>
       </c>
       <c r="B81" t="s">
         <v>381</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>1164</v>
       </c>
       <c r="B82" t="s">
         <v>382</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="D82" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>180</v>
       </c>
       <c r="B83" t="s">
         <v>383</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>610</v>
       </c>
       <c r="B84" t="s">
         <v>384</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="D84" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>1789</v>
       </c>
       <c r="B85" t="s">
         <v>385</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="D85" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>1731</v>
       </c>
       <c r="B86" t="s">
         <v>386</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="D86" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>1045</v>
       </c>
       <c r="B87" t="s">
         <v>387</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="D87" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>619</v>
       </c>
       <c r="B88" t="s">
         <v>388</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="D88" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>1729</v>
       </c>
       <c r="B89" t="s">
         <v>389</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="D89" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>596</v>
       </c>
       <c r="B90" t="s">
         <v>390</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="D90" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>1070</v>
       </c>
       <c r="B91" t="s">
         <v>391</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="D91" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>1141</v>
       </c>
       <c r="B92" t="s">
         <v>392</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="D92" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>2356</v>
       </c>
       <c r="B93" t="s">
         <v>393</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="D93" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>550</v>
       </c>
       <c r="B94" t="s">
         <v>394</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="D94" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>1174</v>
       </c>
       <c r="B95" t="s">
         <v>395</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="D95" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>1193</v>
       </c>
       <c r="B96" t="s">
         <v>396</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="D96" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>1211</v>
       </c>
       <c r="B97" t="s">
         <v>397</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="D97" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>1633</v>
       </c>
       <c r="B98" t="s">
         <v>398</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="D98" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>1075</v>
       </c>
       <c r="B99" t="s">
         <v>399</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="D99" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>1251</v>
       </c>
       <c r="B100" t="s">
         <v>400</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="D100" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>620</v>
       </c>
       <c r="B101" t="s">
         <v>401</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="D101" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>1934</v>
       </c>
       <c r="B102" t="s">
         <v>402</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="D102" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>570</v>
       </c>
       <c r="B103" t="s">
         <v>403</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="D103" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>577</v>
       </c>
       <c r="B104" t="s">
         <v>404</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="D104" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>1661</v>
       </c>
       <c r="B105" t="s">
         <v>405</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="D105" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>197</v>
       </c>
       <c r="B106" t="s">
         <v>406</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="D106" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>1581</v>
       </c>
       <c r="B107" t="s">
         <v>407</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="D107" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>1068</v>
       </c>
       <c r="B108" t="s">
         <v>408</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="D108" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>1378</v>
       </c>
       <c r="B109" t="s">
         <v>409</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="D109" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>1683</v>
       </c>
       <c r="B110" t="s">
         <v>410</v>
       </c>
-      <c r="C110" s="2" t="s">
+      <c r="D110" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>1148</v>
       </c>
       <c r="B111" t="s">
         <v>411</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="D111" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>595</v>
       </c>
       <c r="B112" t="s">
         <v>412</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="D112" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>584</v>
       </c>
       <c r="B113" t="s">
         <v>413</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="D113" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>1757</v>
       </c>
       <c r="B114" t="s">
         <v>414</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="D114" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>721</v>
       </c>
       <c r="B115" t="s">
         <v>415</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="D115" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>1971</v>
       </c>
       <c r="B116" t="s">
         <v>416</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="D116" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>20</v>
       </c>
       <c r="B117" t="s">
         <v>417</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="D117" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>150</v>
       </c>
       <c r="B118" t="s">
         <v>418</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="D118" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>994</v>
       </c>
       <c r="B119" t="s">
         <v>419</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="D119" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>15</v>
       </c>
       <c r="B120" t="s">
         <v>420</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="D120" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>141</v>
       </c>
       <c r="B121" t="s">
         <v>421</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="D121" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>139</v>
       </c>
       <c r="B122" t="s">
         <v>422</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="D122" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>133</v>
       </c>
       <c r="B123" t="s">
         <v>423</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="D123" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>5</v>
       </c>
       <c r="B124" t="s">
         <v>424</v>
       </c>
-      <c r="C124" s="2" t="s">
+      <c r="D124" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>3</v>
       </c>
       <c r="B125" t="s">
         <v>425</v>
       </c>
-      <c r="C125" s="2" t="s">
+      <c r="D125" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>11</v>
       </c>
       <c r="B126" t="s">
         <v>426</v>
       </c>
-      <c r="C126" s="2" t="s">
+      <c r="D126" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>8</v>
       </c>
       <c r="B127" t="s">
         <v>427</v>
       </c>
-      <c r="C127" s="2" t="s">
+      <c r="D127" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>383</v>
       </c>
       <c r="B128" t="s">
         <v>428</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="D128" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>1</v>
       </c>
       <c r="B129" t="s">
         <v>429</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="D129" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>981</v>
       </c>
       <c r="B130" t="s">
         <v>430</v>
       </c>
-      <c r="C130" s="2" t="s">
+      <c r="D130" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>542</v>
       </c>
       <c r="B131" t="s">
         <v>431</v>
       </c>
-      <c r="C131" s="2" t="s">
+      <c r="D131" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>232</v>
       </c>
       <c r="B132" t="s">
         <v>432</v>
       </c>
-      <c r="C132" s="2" t="s">
+      <c r="D132" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>733</v>
       </c>
       <c r="B133" t="s">
         <v>433</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="D133" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>704</v>
       </c>
       <c r="B134" t="s">
         <v>434</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="D134" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>409</v>
       </c>
       <c r="B135" t="s">
         <v>435</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="D135" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>278</v>
       </c>
       <c r="B136" t="s">
         <v>436</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="D136" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>207</v>
       </c>
       <c r="B137" t="s">
         <v>437</v>
       </c>
-      <c r="C137" s="2" t="s">
+      <c r="D137" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>57</v>
       </c>
       <c r="B138" t="s">
         <v>438</v>
       </c>
-      <c r="C138" s="2" t="s">
+      <c r="D138" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>56</v>
       </c>
       <c r="B139" t="s">
         <v>439</v>
       </c>
-      <c r="C139" s="2" t="s">
+      <c r="D139" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>417</v>
       </c>
       <c r="B140" t="s">
         <v>440</v>
       </c>
-      <c r="C140" s="2" t="s">
+      <c r="D140" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>200</v>
       </c>
       <c r="B141" t="s">
         <v>441</v>
       </c>
-      <c r="C141" s="2" t="s">
+      <c r="D141" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>347</v>
       </c>
       <c r="B142" t="s">
         <v>442</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="D142" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>23</v>
       </c>
       <c r="B143" t="s">
         <v>443</v>
       </c>
-      <c r="C143" s="2" t="s">
+      <c r="D143" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>398</v>
       </c>
       <c r="B144" t="s">
         <v>444</v>
       </c>
-      <c r="C144" s="2" t="s">
+      <c r="D144" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>300</v>
       </c>
       <c r="B145" t="s">
         <v>445</v>
       </c>
-      <c r="C145" s="2" t="s">
+      <c r="D145" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>55</v>
       </c>
       <c r="B146" t="s">
         <v>446</v>
       </c>
-      <c r="C146" s="2" t="s">
+      <c r="D146" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>377</v>
       </c>
       <c r="B147" t="s">
         <v>447</v>
       </c>
-      <c r="C147" s="2" t="s">
+      <c r="D147" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>53</v>
       </c>
       <c r="B148" t="s">
         <v>448</v>
       </c>
-      <c r="C148" s="2" t="s">
+      <c r="D148" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>128</v>
       </c>
       <c r="B149" t="s">
         <v>449</v>
       </c>
-      <c r="C149" s="2" t="s">
+      <c r="D149" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>199</v>
       </c>
       <c r="B150" t="s">
         <v>450</v>
       </c>
-      <c r="C150" s="2" t="s">
+      <c r="D150" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>1372</v>
       </c>
       <c r="B151" t="s">
         <v>451</v>
       </c>
-      <c r="C151" s="2" t="s">
+      <c r="D151" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>437</v>
       </c>
       <c r="B152" t="s">
         <v>452</v>
       </c>
-      <c r="C152" s="2" t="s">
+      <c r="D152" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>1448</v>
       </c>
       <c r="B153" t="s">
         <v>453</v>
       </c>
-      <c r="C153" s="2" t="s">
+      <c r="D153" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>100</v>
       </c>
       <c r="B154" t="s">
         <v>454</v>
       </c>
-      <c r="C154" s="2" t="s">
+      <c r="D154" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>2130</v>
       </c>
       <c r="B155" t="s">
         <v>455</v>
       </c>
-      <c r="C155" s="2" t="s">
+      <c r="D155" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>328</v>
       </c>
       <c r="B156" t="s">
         <v>456</v>
       </c>
-      <c r="C156" s="2" t="s">
+      <c r="D156" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>933</v>
       </c>
       <c r="B157" t="s">
         <v>457</v>
       </c>
-      <c r="C157" s="2" t="s">
+      <c r="D157" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>394</v>
       </c>
       <c r="B158" t="s">
         <v>458</v>
       </c>
-      <c r="C158" s="2" t="s">
+      <c r="D158" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>2390</v>
       </c>
       <c r="B159" t="s">
         <v>459</v>
       </c>
-      <c r="C159" s="2" t="s">
+      <c r="D159" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>2352</v>
       </c>
       <c r="B160" t="s">
         <v>460</v>
       </c>
-      <c r="C160" s="2" t="s">
+      <c r="D160" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>1657</v>
       </c>
       <c r="B161" t="s">
         <v>461</v>
       </c>
-      <c r="C161" s="2" t="s">
+      <c r="D161" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>1207</v>
       </c>
       <c r="B162" t="s">
         <v>462</v>
       </c>
-      <c r="C162" s="2" t="s">
+      <c r="D162" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>2215</v>
       </c>
       <c r="B163" t="s">
         <v>463</v>
       </c>
-      <c r="C163" s="2" t="s">
+      <c r="D163" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>1493</v>
       </c>
       <c r="B164" t="s">
         <v>464</v>
       </c>
-      <c r="C164" s="2" t="s">
+      <c r="D164" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>485</v>
       </c>
       <c r="B165" t="s">
         <v>465</v>
       </c>
-      <c r="C165" s="2" t="s">
+      <c r="D165" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>1456</v>
       </c>
       <c r="B166" t="s">
         <v>466</v>
       </c>
-      <c r="C166" s="2" t="s">
+      <c r="D166" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>1679</v>
       </c>
       <c r="B167" t="s">
         <v>467</v>
       </c>
-      <c r="C167" s="2" t="s">
+      <c r="D167" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>121</v>
       </c>
       <c r="B168" t="s">
         <v>468</v>
       </c>
-      <c r="C168" s="2" t="s">
+      <c r="D168" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>144</v>
       </c>
       <c r="B169" t="s">
         <v>469</v>
       </c>
-      <c r="C169" s="2" t="s">
+      <c r="D169" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>572</v>
       </c>
       <c r="B170" t="s">
         <v>470</v>
       </c>
-      <c r="C170" s="2" t="s">
+      <c r="D170" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>102</v>
       </c>
       <c r="B171" t="s">
         <v>471</v>
       </c>
-      <c r="C171" s="2" t="s">
+      <c r="D171" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>226</v>
       </c>
       <c r="B172" t="s">
         <v>472</v>
       </c>
-      <c r="C172" s="2" t="s">
+      <c r="D172" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>104</v>
       </c>
       <c r="B173" t="s">
         <v>473</v>
       </c>
-      <c r="C173" s="2" t="s">
+      <c r="D173" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>647</v>
       </c>
       <c r="B174" t="s">
         <v>474</v>
       </c>
-      <c r="C174" s="2" t="s">
+      <c r="D174" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>49</v>
       </c>
       <c r="B175" t="s">
         <v>475</v>
       </c>
-      <c r="C175" s="2" t="s">
+      <c r="D175" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>242</v>
       </c>
       <c r="B176" t="s">
         <v>476</v>
       </c>
-      <c r="C176" s="2" t="s">
+      <c r="D176" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>48</v>
       </c>
       <c r="B177" t="s">
         <v>477</v>
       </c>
-      <c r="C177" s="2" t="s">
+      <c r="D177" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>54</v>
       </c>
       <c r="B178" t="s">
         <v>478</v>
       </c>
-      <c r="C178" s="2" t="s">
+      <c r="D178" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>19</v>
       </c>
       <c r="B179" t="s">
         <v>479</v>
       </c>
-      <c r="C179" s="2" t="s">
+      <c r="D179" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>206</v>
       </c>
       <c r="B180" t="s">
         <v>480</v>
       </c>
-      <c r="C180" s="2" t="s">
+      <c r="D180" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>1161</v>
       </c>
       <c r="B181" t="s">
         <v>481</v>
       </c>
-      <c r="C181" s="2" t="s">
+      <c r="D181" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>236</v>
       </c>
       <c r="B182" t="s">
         <v>482</v>
       </c>
-      <c r="C182" s="2" t="s">
+      <c r="D182" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>872</v>
       </c>
       <c r="B183" t="s">
         <v>483</v>
       </c>
-      <c r="C183" s="2" t="s">
+      <c r="D183" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>125</v>
       </c>
       <c r="B184" t="s">
         <v>484</v>
       </c>
-      <c r="C184" s="2" t="s">
+      <c r="D184" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>209</v>
       </c>
       <c r="B185" t="s">
         <v>485</v>
       </c>
-      <c r="C185" s="2" t="s">
+      <c r="D185" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>560</v>
       </c>
       <c r="B186" t="s">
         <v>486</v>
       </c>
-      <c r="C186" s="2" t="s">
+      <c r="D186" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>493</v>
       </c>
       <c r="B187" t="s">
         <v>487</v>
       </c>
-      <c r="C187" s="2" t="s">
+      <c r="D187" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>229</v>
       </c>
       <c r="B188" t="s">
         <v>488</v>
       </c>
-      <c r="C188" s="2" t="s">
+      <c r="D188" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>169</v>
       </c>
       <c r="B189" t="s">
         <v>489</v>
       </c>
-      <c r="C189" s="2" t="s">
+      <c r="D189" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>74</v>
       </c>
       <c r="B190" t="s">
         <v>490</v>
       </c>
-      <c r="C190" s="2" t="s">
+      <c r="D190" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>287</v>
       </c>
       <c r="B191" t="s">
         <v>491</v>
       </c>
-      <c r="C191" s="2" t="s">
+      <c r="D191" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>118</v>
       </c>
       <c r="B192" t="s">
         <v>492</v>
       </c>
-      <c r="C192" s="2" t="s">
+      <c r="D192" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>31</v>
       </c>
       <c r="B193" t="s">
         <v>493</v>
       </c>
-      <c r="C193" s="2" t="s">
+      <c r="D193" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>2099</v>
       </c>
       <c r="B194" t="s">
         <v>494</v>
       </c>
-      <c r="C194" s="2" t="s">
+      <c r="D194" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>27</v>
       </c>
       <c r="B195" t="s">
         <v>495</v>
       </c>
-      <c r="C195" s="2" t="s">
+      <c r="D195" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>35</v>
       </c>
       <c r="B196" t="s">
         <v>496</v>
       </c>
-      <c r="C196" s="2" t="s">
+      <c r="D196" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>79</v>
       </c>
       <c r="B197" t="s">
         <v>497</v>
       </c>
-      <c r="C197" s="2" t="s">
+      <c r="D197" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>22</v>
       </c>
       <c r="B198" t="s">
         <v>498</v>
       </c>
-      <c r="C198" s="2" t="s">
+      <c r="D198" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>46</v>
       </c>
       <c r="B199" t="s">
         <v>499</v>
       </c>
-      <c r="C199" s="2" t="s">
+      <c r="D199" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>77</v>
       </c>
       <c r="B200" t="s">
         <v>500</v>
       </c>
-      <c r="C200" s="2" t="s">
+      <c r="D200" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>36</v>
       </c>
       <c r="B201" t="s">
         <v>501</v>
       </c>
-      <c r="C201" s="2" t="s">
+      <c r="D201" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>211</v>
       </c>
       <c r="B202" t="s">
         <v>502</v>
       </c>
-      <c r="C202" s="2" t="s">
+      <c r="D202" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>80</v>
       </c>
       <c r="B203" t="s">
         <v>503</v>
       </c>
-      <c r="C203" s="2" t="s">
+      <c r="D203" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>202</v>
       </c>
       <c r="B204" t="s">
         <v>504</v>
       </c>
-      <c r="C204" s="2" t="s">
+      <c r="D204" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>130</v>
       </c>
       <c r="B205" t="s">
         <v>505</v>
       </c>
-      <c r="C205" s="2" t="s">
+      <c r="D205" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>98</v>
       </c>
       <c r="B206" t="s">
         <v>506</v>
       </c>
-      <c r="C206" s="2" t="s">
+      <c r="D206" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>103</v>
       </c>
       <c r="B207" t="s">
         <v>507</v>
       </c>
-      <c r="C207" s="2" t="s">
+      <c r="D207" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>129</v>
       </c>
       <c r="B208" t="s">
         <v>508</v>
       </c>
-      <c r="C208" s="2" t="s">
+      <c r="D208" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>112</v>
       </c>
       <c r="B209" t="s">
         <v>509</v>
       </c>
-      <c r="C209" s="2" t="s">
+      <c r="D209" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>117</v>
       </c>
       <c r="B210" t="s">
         <v>510</v>
       </c>
-      <c r="C210" s="2" t="s">
+      <c r="D210" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>114</v>
       </c>
       <c r="B211" t="s">
         <v>511</v>
       </c>
-      <c r="C211" s="2" t="s">
+      <c r="D211" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>106</v>
       </c>
       <c r="B212" t="s">
         <v>512</v>
       </c>
-      <c r="C212" s="2" t="s">
+      <c r="D212" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>105</v>
       </c>
       <c r="B213" t="s">
         <v>513</v>
       </c>
-      <c r="C213" s="2" t="s">
+      <c r="D213" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>153</v>
       </c>
       <c r="B214" t="s">
         <v>514</v>
       </c>
-      <c r="C214" s="2" t="s">
+      <c r="D214" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>86</v>
       </c>
       <c r="B215" t="s">
         <v>515</v>
       </c>
-      <c r="C215" s="2" t="s">
+      <c r="D215" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>61</v>
       </c>
       <c r="B216" t="s">
         <v>516</v>
       </c>
-      <c r="C216" s="2" t="s">
+      <c r="D216" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>82</v>
       </c>
       <c r="B217" t="s">
         <v>517</v>
       </c>
-      <c r="C217" s="2" t="s">
+      <c r="D217" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>83</v>
       </c>
       <c r="B218" t="s">
         <v>518</v>
       </c>
-      <c r="C218" s="2" t="s">
+      <c r="D218" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>92</v>
       </c>
       <c r="B219" t="s">
         <v>519</v>
       </c>
-      <c r="C219" s="2" t="s">
+      <c r="D219" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>138</v>
       </c>
       <c r="B220" t="s">
         <v>520</v>
       </c>
-      <c r="C220" s="2" t="s">
+      <c r="D220" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>2</v>
       </c>
       <c r="B221" t="s">
         <v>521</v>
       </c>
-      <c r="C221" s="2" t="s">
+      <c r="D221" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>71</v>
       </c>
       <c r="B222" t="s">
         <v>522</v>
       </c>
-      <c r="C222" s="2" t="s">
+      <c r="D222" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>289</v>
       </c>
       <c r="B223" t="s">
         <v>523</v>
       </c>
-      <c r="C223" s="2" t="s">
+      <c r="D223" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>167</v>
       </c>
       <c r="B224" t="s">
         <v>524</v>
       </c>
-      <c r="C224" s="2" t="s">
+      <c r="D224" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>238</v>
       </c>
       <c r="B225" t="s">
         <v>525</v>
       </c>
-      <c r="C225" s="2" t="s">
+      <c r="D225" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>45</v>
       </c>
       <c r="B226" t="s">
         <v>526</v>
       </c>
-      <c r="C226" s="2" t="s">
+      <c r="D226" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>189</v>
       </c>
       <c r="B227" t="s">
         <v>527</v>
       </c>
-      <c r="C227" s="2" t="s">
+      <c r="D227" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>108</v>
       </c>
       <c r="B228" t="s">
         <v>528</v>
       </c>
-      <c r="C228" s="2" t="s">
+      <c r="D228" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>783</v>
       </c>
       <c r="B229" t="s">
         <v>529</v>
       </c>
-      <c r="C229" s="2" t="s">
+      <c r="D229" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>530</v>
       </c>
       <c r="B230" t="s">
         <v>530</v>
       </c>
-      <c r="C230" s="2" t="s">
+      <c r="D230" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>637</v>
       </c>
       <c r="B231" t="s">
         <v>531</v>
       </c>
-      <c r="C231" s="2" t="s">
+      <c r="D231" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>222</v>
       </c>
       <c r="B232" t="s">
         <v>532</v>
       </c>
-      <c r="C232" s="2" t="s">
+      <c r="D232" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>101</v>
       </c>
       <c r="B233" t="s">
         <v>533</v>
       </c>
-      <c r="C233" s="2" t="s">
+      <c r="D233" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>66</v>
       </c>
       <c r="B234" t="s">
         <v>534</v>
       </c>
-      <c r="C234" s="2" t="s">
+      <c r="D234" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>191</v>
       </c>
       <c r="B235" t="s">
         <v>535</v>
       </c>
-      <c r="C235" s="2" t="s">
+      <c r="D235" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>190</v>
       </c>
       <c r="B236" t="s">
         <v>536</v>
       </c>
-      <c r="C236" s="2" t="s">
+      <c r="D236" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>228</v>
       </c>
       <c r="B237" t="s">
         <v>537</v>
       </c>
-      <c r="C237" s="2" t="s">
+      <c r="D237" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>219</v>
       </c>
       <c r="B238" t="s">
         <v>538</v>
       </c>
-      <c r="C238" s="2" t="s">
+      <c r="D238" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>290</v>
       </c>
       <c r="B239" t="s">
         <v>539</v>
       </c>
-      <c r="C239" s="2" t="s">
+      <c r="D239" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>205</v>
       </c>
       <c r="B240" t="s">
         <v>540</v>
       </c>
-      <c r="C240" s="2" t="s">
+      <c r="D240" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>58</v>
       </c>
       <c r="B241" t="s">
         <v>541</v>
       </c>
-      <c r="C241" s="2" t="s">
+      <c r="D241" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>134</v>
       </c>
       <c r="B242" t="s">
         <v>542</v>
       </c>
-      <c r="C242" s="2" t="s">
+      <c r="D242" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>427</v>
       </c>
       <c r="B243" t="s">
         <v>543</v>
       </c>
-      <c r="C243" s="2" t="s">
+      <c r="D243" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>39</v>
       </c>
       <c r="B244" t="s">
         <v>544</v>
       </c>
-      <c r="C244" s="2" t="s">
+      <c r="D244" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>123</v>
       </c>
       <c r="B245" t="s">
         <v>545</v>
       </c>
-      <c r="C245" s="2" t="s">
+      <c r="D245" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>543</v>
       </c>
       <c r="B246" t="s">
         <v>546</v>
       </c>
-      <c r="C246" s="2" t="s">
+      <c r="D246" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>617</v>
       </c>
       <c r="B247" t="s">
         <v>547</v>
       </c>
-      <c r="C247" s="2" t="s">
+      <c r="D247" s="2" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>501</v>
       </c>
       <c r="B248" t="s">
         <v>548</v>
       </c>
-      <c r="C248" s="2" t="s">
+      <c r="D248" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>563</v>
       </c>
       <c r="B249" t="s">
         <v>549</v>
       </c>
-      <c r="C249" s="2" t="s">
+      <c r="D249" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>463</v>
       </c>
       <c r="B250" t="s">
         <v>550</v>
       </c>
-      <c r="C250" s="2" t="s">
+      <c r="D250" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>404</v>
       </c>
       <c r="B251" t="s">
         <v>551</v>
       </c>
-      <c r="C251" s="2" t="s">
+      <c r="D251" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>257</v>
       </c>
       <c r="B252" t="s">
         <v>552</v>
       </c>
-      <c r="C252" s="2" t="s">
+      <c r="D252" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>201</v>
       </c>
       <c r="B253" t="s">
         <v>553</v>
       </c>
-      <c r="C253" s="2" t="s">
+      <c r="D253" s="2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>137</v>
       </c>
       <c r="B254" t="s">
         <v>554</v>
       </c>
-      <c r="C254" s="2" t="s">
+      <c r="D254" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>274</v>
       </c>
       <c r="B255" t="s">
         <v>555</v>
       </c>
-      <c r="C255" s="2" t="s">
+      <c r="D255" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>148</v>
       </c>
       <c r="B256" t="s">
         <v>556</v>
       </c>
-      <c r="C256" s="2" t="s">
+      <c r="D256" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>912</v>
       </c>
       <c r="B257" t="s">
         <v>557</v>
       </c>
-      <c r="C257" s="2" t="s">
+      <c r="D257" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>718</v>
       </c>
       <c r="B258" t="s">
         <v>558</v>
       </c>
-      <c r="C258" s="2" t="s">
+      <c r="D258" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>172</v>
       </c>
       <c r="B259" t="s">
         <v>559</v>
       </c>
-      <c r="C259" s="2" t="s">
+      <c r="D259" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>373</v>
       </c>
       <c r="B260" t="s">
         <v>560</v>
       </c>
-      <c r="C260" s="2" t="s">
+      <c r="D260" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>227</v>
       </c>
       <c r="B261" t="s">
         <v>561</v>
       </c>
-      <c r="C261" s="2" t="s">
+      <c r="D261" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>155</v>
       </c>
       <c r="B262" t="s">
         <v>562</v>
       </c>
-      <c r="C262" s="2" t="s">
+      <c r="D262" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>2095</v>
       </c>
       <c r="B263" t="s">
         <v>563</v>
       </c>
-      <c r="C263" s="2" t="s">
+      <c r="D263" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>1092</v>
       </c>
       <c r="B264" t="s">
         <v>564</v>
       </c>
-      <c r="C264" s="2" t="s">
+      <c r="D264" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>1084</v>
       </c>
       <c r="B265" t="s">
         <v>565</v>
       </c>
-      <c r="C265" s="2" t="s">
+      <c r="D265" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>1050</v>
       </c>
       <c r="B266" t="s">
         <v>566</v>
       </c>
-      <c r="C266" s="2" t="s">
+      <c r="D266" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>608</v>
       </c>
       <c r="B267" t="s">
         <v>567</v>
       </c>
-      <c r="C267" s="2" t="s">
+      <c r="D267" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>607</v>
       </c>
       <c r="B268" t="s">
         <v>568</v>
       </c>
-      <c r="C268" s="2" t="s">
+      <c r="D268" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>586</v>
       </c>
       <c r="B269" t="s">
         <v>569</v>
       </c>
-      <c r="C269" s="2" t="s">
+      <c r="D269" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>511</v>
       </c>
       <c r="B270" t="s">
         <v>570</v>
       </c>
-      <c r="C270" s="2" t="s">
+      <c r="D270" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>2891</v>
       </c>
       <c r="B271" t="s">
         <v>571</v>
       </c>
-      <c r="C271" s="2" t="s">
+      <c r="D271" s="2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>2890</v>
       </c>
       <c r="B272" t="s">
         <v>572</v>
       </c>
-      <c r="C272" s="2" t="s">
+      <c r="D272" s="2" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>2889</v>
       </c>
       <c r="B273" t="s">
         <v>573</v>
       </c>
-      <c r="C273" s="2" t="s">
+      <c r="D273" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>2888</v>
       </c>
       <c r="B274" t="s">
         <v>574</v>
       </c>
-      <c r="C274" s="2" t="s">
+      <c r="D274" s="2" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>2887</v>
       </c>
       <c r="B275" t="s">
         <v>575</v>
       </c>
-      <c r="C275" s="2" t="s">
+      <c r="D275" s="2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>2886</v>
       </c>
       <c r="B276" t="s">
         <v>576</v>
       </c>
-      <c r="C276" s="2" t="s">
+      <c r="D276" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>2885</v>
       </c>
       <c r="B277" t="s">
         <v>577</v>
       </c>
-      <c r="C277" s="2" t="s">
+      <c r="D277" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>2884</v>
       </c>
       <c r="B278" t="s">
         <v>578</v>
       </c>
-      <c r="C278" s="2" t="s">
+      <c r="D278" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>2883</v>
       </c>
       <c r="B279" t="s">
         <v>579</v>
       </c>
-      <c r="C279" s="2" t="s">
+      <c r="D279" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>2882</v>
       </c>
       <c r="B280" t="s">
         <v>580</v>
       </c>
-      <c r="C280" s="2" t="s">
+      <c r="D280" s="2" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>2881</v>
       </c>
       <c r="B281" t="s">
         <v>581</v>
       </c>
-      <c r="C281" s="2" t="s">
+      <c r="D281" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>2880</v>
       </c>
       <c r="B282" t="s">
         <v>582</v>
       </c>
-      <c r="C282" s="2" t="s">
+      <c r="D282" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>2879</v>
       </c>
       <c r="B283" t="s">
         <v>583</v>
       </c>
-      <c r="C283" s="2" t="s">
+      <c r="D283" s="2" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>2878</v>
       </c>
       <c r="B284" t="s">
         <v>584</v>
       </c>
-      <c r="C284" s="2" t="s">
+      <c r="D284" s="2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>2877</v>
       </c>
       <c r="B285" t="s">
         <v>585</v>
       </c>
-      <c r="C285" s="2" t="s">
+      <c r="D285" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>1517</v>
       </c>
       <c r="B286" t="s">
         <v>586</v>
       </c>
-      <c r="C286" s="2" t="s">
+      <c r="D286" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>1327</v>
       </c>
       <c r="B287" t="s">
         <v>587</v>
       </c>
-      <c r="C287" s="2" t="s">
+      <c r="D287" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>1484</v>
       </c>
       <c r="B288" t="s">
         <v>588</v>
       </c>
-      <c r="C288" s="2" t="s">
+      <c r="D288" s="2" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>176</v>
       </c>
       <c r="B289" t="s">
         <v>589</v>
       </c>
-      <c r="C289" s="2" t="s">
+      <c r="D289" s="2" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>196</v>
       </c>
       <c r="B290" t="s">
         <v>590</v>
       </c>
-      <c r="C290" s="2" t="s">
+      <c r="D290" s="2" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>50</v>
       </c>
       <c r="B291" t="s">
         <v>606</v>
       </c>
-      <c r="C291" s="2" t="s">
+      <c r="D291" s="2" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>1280</v>
       </c>
       <c r="B292" t="s">
         <v>591</v>
       </c>
-      <c r="C292" s="2" t="s">
+      <c r="D292" s="2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>268</v>
       </c>
       <c r="B293" t="s">
         <v>592</v>
       </c>
-      <c r="C293" s="2" t="s">
+      <c r="D293" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>217</v>
       </c>
       <c r="B294" t="s">
         <v>593</v>
       </c>
-      <c r="C294" s="2" t="s">
+      <c r="D294" s="2" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>235</v>
       </c>
       <c r="B295" t="s">
         <v>594</v>
       </c>
-      <c r="C295" s="2" t="s">
+      <c r="D295" s="2" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>230</v>
       </c>
       <c r="B296" t="s">
         <v>595</v>
       </c>
-      <c r="C296" s="2" t="s">
+      <c r="D296" s="2" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>213</v>
       </c>
       <c r="B297" t="s">
         <v>596</v>
       </c>
-      <c r="C297" s="2" t="s">
+      <c r="D297" s="2" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>152</v>
       </c>
       <c r="B298" t="s">
         <v>597</v>
       </c>
-      <c r="C298" s="2" t="s">
+      <c r="D298" s="2" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>845</v>
       </c>
       <c r="B299" t="s">
         <v>598</v>
       </c>
-      <c r="C299" s="2" t="s">
+      <c r="C299" t="s">
+        <v>610</v>
+      </c>
+      <c r="D299" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>160</v>
       </c>
       <c r="B300" t="s">
         <v>599</v>
       </c>
-      <c r="C300" s="2" t="s">
+      <c r="C300" t="s">
+        <v>608</v>
+      </c>
+      <c r="D300" s="2" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>119</v>
       </c>
       <c r="B301" t="s">
         <v>600</v>
       </c>
-      <c r="C301" s="2" t="s">
+      <c r="C301" t="s">
+        <v>607</v>
+      </c>
+      <c r="D301" s="2" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>111</v>
       </c>
       <c r="B302" t="s">
         <v>601</v>
       </c>
-      <c r="C302" s="2" t="s">
+      <c r="C302" t="s">
+        <v>607</v>
+      </c>
+      <c r="D302" s="2" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>110</v>
       </c>
       <c r="B303" t="s">
         <v>602</v>
       </c>
-      <c r="C303" s="2" t="s">
+      <c r="C303" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="D303" s="2" t="s">
         <v>301</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{FA5D311D-DDC3-4581-A2D8-22657DCFC30C}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{CD364B74-66E9-40EF-AD98-BF800CF41614}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{408EF5DB-A300-48F7-B91D-2C278E4DDCE6}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{10859659-2FFC-4F11-B6E8-E1EFE82592C5}"/>
-    <hyperlink ref="C18" r:id="rId5" xr:uid="{30D0C916-6170-4947-B39D-12A69E2DE22D}"/>
-    <hyperlink ref="C301" r:id="rId6" xr:uid="{06015420-878E-43C0-B8C4-D2D0F73ADFC7}"/>
-    <hyperlink ref="C300" r:id="rId7" xr:uid="{D05C0EF0-DB50-4898-A973-E8E6F31F206E}"/>
-    <hyperlink ref="C298" r:id="rId8" xr:uid="{F3375F27-1462-408B-9B47-EE31CFD6E918}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{FA5D311D-DDC3-4581-A2D8-22657DCFC30C}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{CD364B74-66E9-40EF-AD98-BF800CF41614}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{408EF5DB-A300-48F7-B91D-2C278E4DDCE6}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{10859659-2FFC-4F11-B6E8-E1EFE82592C5}"/>
+    <hyperlink ref="D18" r:id="rId5" xr:uid="{30D0C916-6170-4947-B39D-12A69E2DE22D}"/>
+    <hyperlink ref="D301" r:id="rId6" xr:uid="{06015420-878E-43C0-B8C4-D2D0F73ADFC7}"/>
+    <hyperlink ref="D300" r:id="rId7" xr:uid="{D05C0EF0-DB50-4898-A973-E8E6F31F206E}"/>
+    <hyperlink ref="D298" r:id="rId8" xr:uid="{F3375F27-1462-408B-9B47-EE31CFD6E918}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{364667B7-4507-449B-A54F-10F17F097F84}"/>
+    <hyperlink ref="D12" r:id="rId10" xr:uid="{4DD335D5-13DB-4353-A990-861CC50D3C9F}"/>
+    <hyperlink ref="D303" r:id="rId11" xr:uid="{788534EC-DD16-4329-B404-9D94FD1912DF}"/>
+    <hyperlink ref="D302" r:id="rId12" xr:uid="{AC4F437F-1D03-47F2-8FE9-2793463B8093}"/>
+    <hyperlink ref="D299" r:id="rId13" xr:uid="{CB3CC037-1BFE-4706-955E-D679A4F2747F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>